<commit_message>
Release Template ProjektDoku 1.1
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Project documentation/ReleasePlan_Template ProjectDocu.xlsx
+++ b/8. Harmonising standards/Create a project/Project documentation/ReleasePlan_Template ProjectDocu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772AC5DD-042B-417F-A6C1-5F6226847D77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73926F96-E8EE-4F2B-8C92-2E8842F48EB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>SAXESS Software GmbH</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Prozedurenverzeichnis, CorporateDesign</t>
   </si>
   <si>
-    <t>In Arbeit</t>
-  </si>
-  <si>
     <t>Release Template ProjektDoku 2.0</t>
   </si>
   <si>
@@ -119,6 +116,24 @@
   </si>
   <si>
     <t>Erweiterung ProjektDoku-Template</t>
+  </si>
+  <si>
+    <t>Erledigt</t>
+  </si>
+  <si>
+    <t>Release Template ProjektDoku 1.1</t>
+  </si>
+  <si>
+    <t>Checkliste &amp; Layout überarbeiten</t>
+  </si>
+  <si>
+    <t>Inhalte Checkliste angepasst und Spalten reduziert</t>
+  </si>
+  <si>
+    <t>SX Logo herausgenommen</t>
+  </si>
+  <si>
+    <t>Header &amp; Spaltenbreiten angepasst</t>
   </si>
 </sst>
 </file>
@@ -334,7 +349,55 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -804,12 +867,12 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BB308"/>
+  <dimension ref="A1:BB311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1160,7 @@
       <c r="M8" s="13"/>
       <c r="N8" s="33"/>
     </row>
-    <row r="9" spans="1:54" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
         <v>2</v>
       </c>
@@ -1114,7 +1177,7 @@
       <c r="M9" s="31"/>
       <c r="N9" s="34"/>
     </row>
-    <row r="10" spans="1:54" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -1122,15 +1185,26 @@
       <c r="M10" s="22"/>
       <c r="N10" s="33"/>
     </row>
-    <row r="11" spans="1:54" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="33"/>
-    </row>
-    <row r="12" spans="1:54" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26">
+        <v>43368</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -1138,23 +1212,47 @@
       <c r="M12" s="22"/>
       <c r="N12" s="33"/>
     </row>
-    <row r="13" spans="1:54" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="22"/>
+    <row r="13" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="20">
+        <v>0</v>
+      </c>
+      <c r="J13" s="20">
+        <v>0</v>
+      </c>
+      <c r="K13" s="20">
+        <f>I13/100*(100-J13)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="M13" s="22"/>
-      <c r="N13" s="33"/>
-    </row>
-    <row r="14" spans="1:54" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="36"/>
+    </row>
+    <row r="14" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
-      <c r="N14" s="33"/>
-    </row>
-    <row r="15" spans="1:54" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="36"/>
+    </row>
+    <row r="15" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
@@ -1162,7 +1260,7 @@
       <c r="M15" s="22"/>
       <c r="N15" s="33"/>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
@@ -1170,22 +1268,24 @@
       <c r="M16" s="22"/>
       <c r="N16" s="33"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="34"/>
+    <row r="17" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26">
+        <v>43369</v>
+      </c>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="35"/>
     </row>
     <row r="18" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I18" s="20"/>
@@ -1196,73 +1296,63 @@
       <c r="N18" s="33"/>
     </row>
     <row r="19" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26">
-        <v>43455</v>
-      </c>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="35"/>
+      <c r="B19" s="18">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="20">
+        <v>0</v>
+      </c>
+      <c r="J19" s="20">
+        <v>0</v>
+      </c>
+      <c r="K19" s="20">
+        <f>I19/100*(100-J19)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="22"/>
+      <c r="N19" s="36"/>
     </row>
     <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
-      <c r="N20" s="33"/>
+      <c r="N20" s="36"/>
     </row>
     <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="18">
-        <v>1</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="20">
-        <v>0</v>
-      </c>
-      <c r="J21" s="20">
-        <v>0</v>
-      </c>
-      <c r="K21" s="20">
-        <f>I21/100*(100-J21)</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="C21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="22"/>
       <c r="M21" s="22"/>
-      <c r="N21" s="36"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
-        <v>20</v>
-      </c>
       <c r="C22" s="19" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
-      <c r="N22" s="36"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="19" t="s">
-        <v>23</v>
-      </c>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
@@ -1271,7 +1361,6 @@
       <c r="N23" s="33"/>
     </row>
     <row r="24" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="19"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
@@ -1279,72 +1368,57 @@
       <c r="M24" s="22"/>
       <c r="N24" s="33"/>
     </row>
-    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="35"/>
-    </row>
-    <row r="26" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="33"/>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="33"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="34"/>
     </row>
     <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
-        <v>1</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I27" s="20">
-        <v>0</v>
-      </c>
-      <c r="J27" s="20">
-        <v>0</v>
-      </c>
-      <c r="K27" s="20">
-        <f>I27/100*(100-J27)</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="22" t="s">
-        <v>17</v>
-      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="22"/>
       <c r="M27" s="22"/>
-      <c r="N27" s="36"/>
+      <c r="N27" s="33"/>
     </row>
     <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="36"/>
+      <c r="B28" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="35"/>
     </row>
     <row r="29" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
@@ -1353,27 +1427,46 @@
       <c r="N29" s="33"/>
     </row>
     <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="18">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="22"/>
+      <c r="I30" s="20">
+        <v>0</v>
+      </c>
+      <c r="J30" s="20">
+        <v>0</v>
+      </c>
+      <c r="K30" s="20">
+        <f>I30/100*(100-J30)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="M30" s="22"/>
-      <c r="N30" s="33"/>
+      <c r="N30" s="36"/>
     </row>
     <row r="31" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="19"/>
+      <c r="B31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
-      <c r="N31" s="33"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C32" s="19"/>
+      <c r="N31" s="36"/>
+    </row>
+    <row r="32" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
@@ -1381,24 +1474,19 @@
       <c r="M32" s="22"/>
       <c r="N32" s="33"/>
     </row>
-    <row r="33" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="34"/>
-    </row>
-    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="33"/>
+    </row>
+    <row r="34" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="19"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
@@ -1406,51 +1494,33 @@
       <c r="M34" s="22"/>
       <c r="N34" s="33"/>
     </row>
-    <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="20">
-        <v>5</v>
-      </c>
-      <c r="J35" s="20">
-        <v>100</v>
-      </c>
-      <c r="K35" s="20">
-        <f>I35/100*(100-J35)</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="M35" s="22">
-        <v>1</v>
-      </c>
-      <c r="N35" s="36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="36" t="s">
-        <v>12</v>
-      </c>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C35" s="19"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="33"/>
+    </row>
+    <row r="36" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="34"/>
     </row>
     <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="19" t="s">
-        <v>14</v>
-      </c>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
@@ -1459,17 +1529,34 @@
       <c r="N37" s="33"/>
     </row>
     <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="33"/>
+      <c r="B38" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="20">
+        <v>5</v>
+      </c>
+      <c r="J38" s="20">
+        <v>100</v>
+      </c>
+      <c r="K38" s="20">
+        <f>I38/100*(100-J38)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" s="22">
+        <v>1</v>
+      </c>
+      <c r="N38" s="36" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="39" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
       <c r="C39" s="19" t="s">
         <v>14</v>
       </c>
@@ -1478,9 +1565,14 @@
       <c r="K39" s="20"/>
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
-      <c r="N39" s="33"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N39" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
       <c r="K40" s="20"/>
@@ -1488,7 +1580,10 @@
       <c r="M40" s="22"/>
       <c r="N40" s="33"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
@@ -1496,7 +1591,10 @@
       <c r="M41" s="22"/>
       <c r="N41" s="33"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
       <c r="K42" s="20"/>
@@ -1505,26 +1603,28 @@
       <c r="N42" s="33"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="37"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="33"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="33"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="33"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I46" s="21"/>
@@ -1532,6 +1632,7 @@
       <c r="K46" s="21"/>
       <c r="L46" s="23"/>
       <c r="M46" s="23"/>
+      <c r="N46" s="37"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I47" s="21"/>
@@ -2846,16 +2947,22 @@
       <c r="I234" s="21"/>
       <c r="J234" s="21"/>
       <c r="K234" s="21"/>
+      <c r="L234" s="23"/>
+      <c r="M234" s="23"/>
     </row>
     <row r="235" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I235" s="21"/>
       <c r="J235" s="21"/>
       <c r="K235" s="21"/>
+      <c r="L235" s="23"/>
+      <c r="M235" s="23"/>
     </row>
     <row r="236" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I236" s="21"/>
       <c r="J236" s="21"/>
       <c r="K236" s="21"/>
+      <c r="L236" s="23"/>
+      <c r="M236" s="23"/>
     </row>
     <row r="237" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I237" s="21"/>
@@ -3217,24 +3324,55 @@
       <c r="J308" s="21"/>
       <c r="K308" s="21"/>
     </row>
+    <row r="309" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I309" s="21"/>
+      <c r="J309" s="21"/>
+      <c r="K309" s="21"/>
+    </row>
+    <row r="310" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I310" s="21"/>
+      <c r="J310" s="21"/>
+      <c r="K310" s="21"/>
+    </row>
+    <row r="311" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I311" s="21"/>
+      <c r="J311" s="21"/>
+      <c r="K311" s="21"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M18:M24 M9:M16 M30:M998">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="M27 M9:M10 M33:M1001 M16 M22:M25">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="M26">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:M29">
+  <conditionalFormatting sqref="M28:M32">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M15">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M21">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>